<commit_message>
modification html et css
</commit_message>
<xml_diff>
--- a/Checklist^MAudit^MSEO^M2018 (2).xlsx
+++ b/Checklist^MAudit^MSEO^M2018 (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1b5709471efc6e4/Desktop/PROJET SEO/Starting^Mwebsite/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="11_246BDC33819B0CABD781BBBDE29A5B5C78A34492" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F43848BB-1C51-4AFE-A72A-9F1F389B0FF5}"/>
+  <xr:revisionPtr revIDLastSave="273" documentId="11_246BDC33819B0CABD781BBBDE29A5B5C78A34492" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3EE9F3D1-1A48-48FA-AF07-6CA70804B905}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>Vérifications</t>
   </si>
@@ -343,6 +343,12 @@
 Ces liens sont utilisés pour donner de l’autorité au site, seulement ils sont contre productifs. Non seulement les liens en footers ne sont pas toujours crawlés par Google mais en plus ils peuvent être considérés comme backlinks. Ce qui est pénalisé par les navigateurs. 
 Nous pouvons conserver les liens vers les annuaires du secteur ainsi que les liens vers les sites partenaires. Néanmoins, cela ne fait pas très sérieux et ne donne pas confiance. </t>
     </r>
+  </si>
+  <si>
+    <t>Minifier le fichier javascript</t>
+  </si>
+  <si>
+    <t>LightHouse</t>
   </si>
 </sst>
 </file>
@@ -634,246 +640,222 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1269,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1285,248 +1267,280 @@
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="16"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="43"/>
     </row>
     <row r="11" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="14" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="43"/>
     </row>
     <row r="15" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="43"/>
     </row>
     <row r="19" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="8"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="32"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="8"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="32"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="16"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="7"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="7"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
@@ -1543,47 +1557,19 @@
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D28">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1599,157 +1585,157 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" style="39" customWidth="1"/>
-    <col min="2" max="2" width="55.6328125" style="76" customWidth="1"/>
+    <col min="1" max="1" width="39" style="7" customWidth="1"/>
+    <col min="2" max="2" width="55.6328125" style="21" customWidth="1"/>
     <col min="3" max="3" width="44.7265625" style="4" customWidth="1"/>
     <col min="4" max="5" width="56.90625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="56.90625" style="39" customWidth="1"/>
-    <col min="7" max="16384" width="14.453125" style="39"/>
+    <col min="6" max="6" width="56.90625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="14.453125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="54" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="56" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="48"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51" t="s">
+      <c r="D5" s="65"/>
+      <c r="E5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="58" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="48"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="57"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45" t="s">
+      <c r="D7" s="64"/>
+      <c r="E7" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="55"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="56"/>
-    </row>
-    <row r="9" spans="1:6" s="61" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A8" s="68"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="60"/>
+    </row>
+    <row r="9" spans="1:6" s="12" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="64" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
+    <row r="10" spans="1:6" s="15" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="76" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="66" t="s">
@@ -1758,45 +1744,45 @@
       <c r="D11" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="67"/>
+      <c r="F11" s="61"/>
     </row>
     <row r="12" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="48"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="68"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="62"/>
     </row>
     <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="48"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="70" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -1805,138 +1791,160 @@
       <c r="C15" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="69"/>
+      <c r="F15" s="63"/>
     </row>
     <row r="16" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="48"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="20" t="s">
+      <c r="D17" s="64"/>
+      <c r="E17" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="F17" s="62" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="48"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="65" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="58" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="48"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="57"/>
     </row>
     <row r="21" spans="1:6" ht="91" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="17" t="s">
         <v>74</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="73"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="71" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="74" t="s">
+      <c r="F23" s="19" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
@@ -1949,61 +1957,39 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="A15:B16 A17:C21 A1:F8 A11:C14 D11:F20 A10:D10 D21:E21">
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C16">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:C9">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:D23">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
pourquoi la performance du site change-t-elle ?
</commit_message>
<xml_diff>
--- a/Checklist^MAudit^MSEO^M2018 (2).xlsx
+++ b/Checklist^MAudit^MSEO^M2018 (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1b5709471efc6e4/Desktop/PROJET SEO/Starting^Mwebsite/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="273" documentId="11_246BDC33819B0CABD781BBBDE29A5B5C78A34492" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3EE9F3D1-1A48-48FA-AF07-6CA70804B905}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="11_246BDC33819B0CABD781BBBDE29A5B5C78A34492" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E6FFD1FF-D1EC-4F20-ADC8-7AC60147E2A0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,111 +691,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -805,49 +832,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -947,6 +947,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>74137</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B18C2E0-0FFC-430F-A47D-BDE8BF2851F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12725400"/>
+          <a:ext cx="7772400" cy="1648937"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9316D283-4CEC-4232-869E-FC818F3F2E62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14693900"/>
+          <a:ext cx="7772400" cy="1943099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,245 +1369,293 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="39"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="43"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="32"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="43"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="32"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="43"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="43"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="32"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="25" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="43"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="32"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="43"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="43"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="32"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="43"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="31"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="32"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="31"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="39"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="34"/>
     </row>
     <row r="29" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="34"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="36"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="34"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="36"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="B21:B22"/>
@@ -1519,54 +1672,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D28">
     <cfRule type="expression" dxfId="9" priority="1">
@@ -1585,8 +1690,8 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1600,110 +1705,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="75" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="55"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="76"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="67" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="57"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="64" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="57"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="62"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="59"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="60"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" s="12" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1732,130 +1837,130 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="61"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="57"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="62"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="62"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="57"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="62"/>
     </row>
     <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66" t="s">
+      <c r="D15" s="52"/>
+      <c r="E15" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="63"/>
+      <c r="F15" s="61"/>
     </row>
     <row r="16" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="57"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="46" t="s">
+      <c r="D17" s="55"/>
+      <c r="E17" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="63" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="57"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="62"/>
     </row>
     <row r="19" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="66" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="66" t="s">
+      <c r="E19" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="58" t="s">
+      <c r="F19" s="64" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="68"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="57"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="1:6" ht="91" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
@@ -1913,39 +2018,11 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="E1:E2"/>
@@ -1962,11 +2039,39 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="A15:B16 A17:C21 A1:F8 A11:C14 D11:F20 A10:D10 D21:E21">
     <cfRule type="expression" dxfId="8" priority="15">
@@ -2019,5 +2124,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>